<commit_message>
More work on spec
</commit_message>
<xml_diff>
--- a/Documentation/diagrams.xlsx
+++ b/Documentation/diagrams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\Microwave-SDR\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BD4286-003C-4DDB-9109-01E6C3DD39BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE9AFD3-80F9-4DF0-B777-703CE7098A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EB6F11D-DA4C-4D3A-9BD8-4D901884D870}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EB6F11D-DA4C-4D3A-9BD8-4D901884D870}"/>
   </bookViews>
   <sheets>
     <sheet name="Card to Baseboard Pinout" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
   <si>
     <t>a</t>
   </si>
@@ -63,36 +63,6 @@
     <t>Address EEPROM</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>SDA</t>
-  </si>
-  <si>
-    <t>SCL</t>
-  </si>
-  <si>
-    <t>ADDR2</t>
-  </si>
-  <si>
-    <t>ADDR1</t>
-  </si>
-  <si>
-    <t>ADDR0</t>
-  </si>
-  <si>
-    <t>3V3_OUT</t>
-  </si>
-  <si>
-    <t>WP</t>
-  </si>
-  <si>
-    <t>3V3_IN</t>
-  </si>
-  <si>
     <t>SMA - REF OSC</t>
   </si>
   <si>
@@ -103,6 +73,48 @@
   </si>
   <si>
     <t>Spare</t>
+  </si>
+  <si>
+    <t>TX_EN</t>
+  </si>
+  <si>
+    <t>GPIO</t>
+  </si>
+  <si>
+    <t>ADDR_SDA</t>
+  </si>
+  <si>
+    <t>ADDR_WP</t>
+  </si>
+  <si>
+    <t>ADDR_SCL</t>
+  </si>
+  <si>
+    <t>ADDR_3V3</t>
+  </si>
+  <si>
+    <t>PSU_3V3</t>
+  </si>
+  <si>
+    <t>PSU_SDA</t>
+  </si>
+  <si>
+    <t>PSU_SCL</t>
+  </si>
+  <si>
+    <t>PSU_ADDR2</t>
+  </si>
+  <si>
+    <t>PSU_ADDR1</t>
+  </si>
+  <si>
+    <t>PSU_ADDR0</t>
+  </si>
+  <si>
+    <t>RS485_B</t>
+  </si>
+  <si>
+    <t>RS485_A</t>
   </si>
 </sst>
 </file>
@@ -306,7 +318,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -332,17 +344,31 @@
     <xf numFmtId="49" fontId="5" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="7" fillId="9" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -669,11 +695,12 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="4" width="12.7109375" customWidth="1"/>
     <col min="7" max="7" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -823,8 +850,8 @@
       <c r="E8" s="3">
         <v>7</v>
       </c>
-      <c r="G8" s="15" t="s">
-        <v>25</v>
+      <c r="G8" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -843,6 +870,9 @@
       <c r="E9" s="3">
         <v>8</v>
       </c>
+      <c r="G9" s="12" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -882,15 +912,9 @@
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>13</v>
-      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="3">
         <v>11</v>
       </c>
@@ -899,14 +923,10 @@
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>12</v>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="E13" s="3">
         <v>12</v>
@@ -916,9 +936,15 @@
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
+      <c r="B14" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="E14" s="3">
         <v>13</v>
       </c>
@@ -927,9 +953,15 @@
       <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
+      <c r="B15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>29</v>
+      </c>
       <c r="E15" s="3">
         <v>14</v>
       </c>
@@ -938,14 +970,14 @@
       <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>15</v>
+      <c r="B16" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="E16" s="3">
         <v>15</v>
@@ -955,14 +987,14 @@
       <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>18</v>
+      <c r="B17" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="E17" s="3">
         <v>16</v>
@@ -982,28 +1014,28 @@
       <c r="E18" s="3"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="13" t="s">
-        <v>22</v>
+      <c r="C21" s="10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="13"/>
+      <c r="C22" s="10"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="12" t="s">
-        <v>23</v>
+      <c r="C24" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="12"/>
+      <c r="C25" s="11"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="12" t="s">
-        <v>24</v>
+      <c r="C27" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="12"/>
+      <c r="C28" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>